<commit_message>
feature: excel 'empresa per mida y provincia' changed and graphics made
</commit_message>
<xml_diff>
--- a/data/Empresa per mida y provincia 2008-2022.xlsx
+++ b/data/Empresa per mida y provincia 2008-2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\miria\OneDrive - Universitat Politècnica de Catalunya\Personal\HACKATON\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{840B89C9-7736-4258-B5FE-BAB9836F4ABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14166926-9E4C-4173-9532-55A365A7965F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{4EEA3490-7564-45D2-A2CA-A64496852BF8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="98">
   <si>
     <t>CCAA</t>
   </si>
@@ -365,11 +365,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -830,8 +829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE9A989E-A2FA-40A6-BE6E-50CA55C495A5}">
   <dimension ref="B1:AE73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" zoomScale="106" zoomScaleNormal="52" workbookViewId="0">
-      <selection activeCell="AG17" sqref="AG17"/>
+    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="106" zoomScaleNormal="52" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -874,13 +873,13 @@
       <c r="D1" t="s">
         <v>84</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>70</v>
       </c>
       <c r="F1" t="s">
         <v>85</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" t="s">
         <v>71</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -928,7 +927,7 @@
       <c r="V1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" t="s">
         <v>79</v>
       </c>
       <c r="X1" s="2" t="s">
@@ -3993,6 +3992,9 @@
       </c>
     </row>
     <row r="35" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
@@ -4082,6 +4084,9 @@
       </c>
     </row>
     <row r="36" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
@@ -4171,6 +4176,9 @@
       </c>
     </row>
     <row r="37" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
       <c r="C37" t="s">
         <v>37</v>
       </c>
@@ -4260,6 +4268,9 @@
       </c>
     </row>
     <row r="38" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>33</v>
+      </c>
       <c r="C38" t="s">
         <v>38</v>
       </c>
@@ -4349,6 +4360,9 @@
       </c>
     </row>
     <row r="39" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>33</v>
+      </c>
       <c r="C39" t="s">
         <v>2</v>
       </c>
@@ -4530,6 +4544,9 @@
       </c>
     </row>
     <row r="41" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>39</v>
+      </c>
       <c r="C41" t="s">
         <v>41</v>
       </c>
@@ -4619,6 +4636,9 @@
       </c>
     </row>
     <row r="42" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
       <c r="C42" t="s">
         <v>42</v>
       </c>
@@ -4708,6 +4728,9 @@
       </c>
     </row>
     <row r="43" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>39</v>
+      </c>
       <c r="C43" t="s">
         <v>43</v>
       </c>
@@ -4797,6 +4820,9 @@
       </c>
     </row>
     <row r="44" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>39</v>
+      </c>
       <c r="C44" t="s">
         <v>2</v>
       </c>
@@ -4978,6 +5004,9 @@
       </c>
     </row>
     <row r="46" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>44</v>
+      </c>
       <c r="C46" t="s">
         <v>2</v>
       </c>
@@ -5159,6 +5188,9 @@
       </c>
     </row>
     <row r="48" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>45</v>
+      </c>
       <c r="C48" t="s">
         <v>47</v>
       </c>
@@ -5248,6 +5280,9 @@
       </c>
     </row>
     <row r="49" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>45</v>
+      </c>
       <c r="C49" t="s">
         <v>48</v>
       </c>
@@ -5337,6 +5372,9 @@
       </c>
     </row>
     <row r="50" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>45</v>
+      </c>
       <c r="C50" t="s">
         <v>2</v>
       </c>
@@ -5518,6 +5556,9 @@
       </c>
     </row>
     <row r="52" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>49</v>
+      </c>
       <c r="C52" t="s">
         <v>51</v>
       </c>
@@ -5607,6 +5648,9 @@
       </c>
     </row>
     <row r="53" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>49</v>
+      </c>
       <c r="C53" t="s">
         <v>2</v>
       </c>
@@ -5788,6 +5832,9 @@
       </c>
     </row>
     <row r="55" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>52</v>
+      </c>
       <c r="C55" t="s">
         <v>54</v>
       </c>
@@ -5877,6 +5924,9 @@
       </c>
     </row>
     <row r="56" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>52</v>
+      </c>
       <c r="C56" t="s">
         <v>55</v>
       </c>
@@ -5966,6 +6016,9 @@
       </c>
     </row>
     <row r="57" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>52</v>
+      </c>
       <c r="C57" t="s">
         <v>56</v>
       </c>
@@ -6055,6 +6108,9 @@
       </c>
     </row>
     <row r="58" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>52</v>
+      </c>
       <c r="C58" t="s">
         <v>2</v>
       </c>
@@ -6236,6 +6292,9 @@
       </c>
     </row>
     <row r="60" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>57</v>
+      </c>
       <c r="C60" t="s">
         <v>2</v>
       </c>
@@ -6417,6 +6476,9 @@
       </c>
     </row>
     <row r="62" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>59</v>
+      </c>
       <c r="C62" t="s">
         <v>2</v>
       </c>
@@ -6598,6 +6660,9 @@
       </c>
     </row>
     <row r="64" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>60</v>
+      </c>
       <c r="C64" t="s">
         <v>2</v>
       </c>
@@ -6779,6 +6844,9 @@
       </c>
     </row>
     <row r="66" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>62</v>
+      </c>
       <c r="C66" t="s">
         <v>2</v>
       </c>
@@ -6960,6 +7028,9 @@
       </c>
     </row>
     <row r="68" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>64</v>
+      </c>
       <c r="C68" t="s">
         <v>66</v>
       </c>
@@ -7049,6 +7120,9 @@
       </c>
     </row>
     <row r="69" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>64</v>
+      </c>
       <c r="C69" t="s">
         <v>67</v>
       </c>
@@ -7138,6 +7212,9 @@
       </c>
     </row>
     <row r="70" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>64</v>
+      </c>
       <c r="C70" t="s">
         <v>2</v>
       </c>
@@ -7319,6 +7396,9 @@
       </c>
     </row>
     <row r="72" spans="2:31" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>68</v>
+      </c>
       <c r="C72" t="s">
         <v>2</v>
       </c>

</xml_diff>